<commit_message>
reads header row to find which columns hold what
</commit_message>
<xml_diff>
--- a/resources/files/test1.xlsx
+++ b/resources/files/test1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17csc\eclipse-workspace\harlam-ozeret\resources\files\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,27 +24,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Bunk</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Bunk</t>
+    <t>Cooper</t>
   </si>
   <si>
     <t>On Time</t>
   </si>
   <si>
-    <t>Cooper</t>
-  </si>
-  <si>
-    <t>SB1</t>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Late</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -356,34 +363,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some pre-filled values to make testing easier, started creation of unaccounted-for staff list (right now just lists all staff by bunk)
</commit_message>
<xml_diff>
--- a/resources/files/test1.xlsx
+++ b/resources/files/test1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17csc\eclipse-workspace\harlam-ozeret\resources\files\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -51,7 +51,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,7 +365,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -392,9 +391,6 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>

</xml_diff>